<commit_message>
Modified readwriter, entity and fixed given excel sheet
</commit_message>
<xml_diff>
--- a/database/staff_list.xlsx
+++ b/database/staff_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2023S1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elain\Documents\2)NTU Uni\2_year2\y2s1\2) SC2002 Object Oriented Design and Programming\sc2002Assignment\sc2002-project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD0A763-F36A-4773-B526-842599E71A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E2DFEC-8B67-4077-94FA-0134F4EAD761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="staff" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$1:$B$88</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$1:$B$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">staff!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -95,7 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,23 +117,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="64"/>
-      <name val="Microsoft Sans Serif"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Microsoft Sans Serif"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Microsoft Sans Serif"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="8"/>
       <color indexed="64"/>
@@ -146,12 +129,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Microsoft Sans Serif"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -181,23 +158,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,22 +482,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" style="7" customWidth="1"/>
+    <col min="1" max="1" width="22" style="4" customWidth="1"/>
     <col min="2" max="2" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -542,7 +511,7 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
@@ -553,7 +522,7 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
@@ -564,7 +533,7 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
@@ -575,7 +544,7 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
@@ -586,318 +555,12 @@
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="4"/>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="4"/>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="4"/>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="4"/>
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="4"/>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="4"/>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="4"/>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="4"/>
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="4"/>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="9"/>
-      <c r="B62" s="10"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="2"/>
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="2"/>
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="4"/>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
-      <c r="B72" s="2"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
-      <c r="B73" s="2"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="4"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="4"/>
-      <c r="B75" s="2"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
-      <c r="B76" s="2"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="3"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="3"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="3"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added DateRange + Project Structure Changes
</commit_message>
<xml_diff>
--- a/database/staff_list.xlsx
+++ b/database/staff_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elain\Documents\2)NTU Uni\2_year2\y2s1\2) SC2002 Object Oriented Design and Programming\sc2002Assignment\sc2002-project\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sengy\Desktop\Workspace\School\NTU\SC2002 (OOP)\sc2002-project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E2DFEC-8B67-4077-94FA-0134F4EAD761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9450597D-285C-4255-A7D4-F4CD7189D49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
   <sheets>
     <sheet name="staff" sheetId="1" r:id="rId1"/>
@@ -64,18 +64,12 @@
     <t>Madhukumar</t>
   </si>
   <si>
-    <t xml:space="preserve">Alexei </t>
-  </si>
-  <si>
     <t>Chattopadhyay</t>
   </si>
   <si>
     <t>Datta</t>
   </si>
   <si>
-    <t xml:space="preserve">Arvind </t>
-  </si>
-  <si>
     <t>ARVI@NTU.EDU.SG</t>
   </si>
   <si>
@@ -89,6 +83,12 @@
   </si>
   <si>
     <t>HUKUMAR@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>Alexei</t>
+  </si>
+  <si>
+    <t>Arvind</t>
   </si>
 </sst>
 </file>
@@ -487,16 +487,16 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD166"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -507,56 +507,56 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>

</xml_diff>